<commit_message>
Updated Emission factors and plots
</commit_message>
<xml_diff>
--- a/model_outputs/impacts/reductions.xlsx
+++ b/model_outputs/impacts/reductions.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24026"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://gtvault-my.sharepoint.com/personal/obroesicke3_gatech_edu/Documents/00_PhD/GitHub/DistributedEnergyGen/model_outputs/impacts/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="77" documentId="8_{D10A294E-E8C7-4A00-AE8A-00FCE5A3AFD0}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{BC7B997F-5B24-4902-9DB1-900068CC9097}"/>
+  <xr:revisionPtr revIDLastSave="77" documentId="8_{D10A294E-E8C7-4A00-AE8A-00FCE5A3AFD0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{BC7B997F-5B24-4902-9DB1-900068CC9097}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{32BF44EB-935B-4F4B-BDC1-B755049E81DC}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{32BF44EB-935B-4F4B-BDC1-B755049E81DC}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -260,41 +260,41 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="2" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="2" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="2" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="2" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -617,7 +617,7 @@
       <pane xSplit="5" ySplit="3" topLeftCell="H4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="F1" sqref="F1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="AG22" sqref="AG22"/>
+      <selection pane="bottomRight" activeCell="U20" sqref="U20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -669,64 +669,64 @@
       </c>
     </row>
     <row r="2" spans="1:39" x14ac:dyDescent="0.25">
-      <c r="F2" s="27" t="s">
+      <c r="F2" s="24" t="s">
         <v>26</v>
       </c>
-      <c r="G2" s="25" t="s">
+      <c r="G2" s="30" t="s">
         <v>10</v>
       </c>
-      <c r="H2" s="25"/>
-      <c r="I2" s="25"/>
-      <c r="J2" s="25" t="s">
+      <c r="H2" s="30"/>
+      <c r="I2" s="30"/>
+      <c r="J2" s="30" t="s">
         <v>11</v>
       </c>
-      <c r="K2" s="25"/>
-      <c r="L2" s="25"/>
-      <c r="M2" s="25" t="s">
+      <c r="K2" s="30"/>
+      <c r="L2" s="30"/>
+      <c r="M2" s="30" t="s">
         <v>12</v>
       </c>
-      <c r="N2" s="25"/>
-      <c r="O2" s="25"/>
-      <c r="P2" s="25" t="s">
+      <c r="N2" s="30"/>
+      <c r="O2" s="30"/>
+      <c r="P2" s="30" t="s">
         <v>13</v>
       </c>
-      <c r="Q2" s="25"/>
-      <c r="R2" s="25"/>
-      <c r="S2" s="25" t="s">
+      <c r="Q2" s="30"/>
+      <c r="R2" s="30"/>
+      <c r="S2" s="30" t="s">
         <v>14</v>
       </c>
-      <c r="T2" s="25"/>
-      <c r="U2" s="25"/>
-      <c r="V2" s="25" t="s">
+      <c r="T2" s="30"/>
+      <c r="U2" s="30"/>
+      <c r="V2" s="30" t="s">
         <v>15</v>
       </c>
-      <c r="W2" s="25"/>
-      <c r="X2" s="25"/>
-      <c r="Y2" s="25" t="s">
+      <c r="W2" s="30"/>
+      <c r="X2" s="30"/>
+      <c r="Y2" s="30" t="s">
         <v>16</v>
       </c>
-      <c r="Z2" s="25"/>
-      <c r="AA2" s="25"/>
-      <c r="AB2" s="25" t="s">
+      <c r="Z2" s="30"/>
+      <c r="AA2" s="30"/>
+      <c r="AB2" s="30" t="s">
         <v>17</v>
       </c>
-      <c r="AC2" s="25"/>
-      <c r="AD2" s="25"/>
-      <c r="AE2" s="25" t="s">
+      <c r="AC2" s="30"/>
+      <c r="AD2" s="30"/>
+      <c r="AE2" s="30" t="s">
         <v>18</v>
       </c>
-      <c r="AF2" s="25"/>
-      <c r="AG2" s="25"/>
-      <c r="AH2" s="25" t="s">
+      <c r="AF2" s="30"/>
+      <c r="AG2" s="30"/>
+      <c r="AH2" s="30" t="s">
         <v>19</v>
       </c>
-      <c r="AI2" s="25"/>
-      <c r="AJ2" s="25"/>
-      <c r="AK2" s="25" t="s">
+      <c r="AI2" s="30"/>
+      <c r="AJ2" s="30"/>
+      <c r="AK2" s="30" t="s">
         <v>20</v>
       </c>
-      <c r="AL2" s="25"/>
-      <c r="AM2" s="25"/>
+      <c r="AL2" s="30"/>
+      <c r="AM2" s="30"/>
     </row>
     <row r="3" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
@@ -744,7 +744,7 @@
       <c r="E3" t="s">
         <v>25</v>
       </c>
-      <c r="F3" s="28"/>
+      <c r="F3" s="25"/>
       <c r="G3" s="1" t="s">
         <v>21</v>
       </c>
@@ -846,10 +846,10 @@
       </c>
     </row>
     <row r="4" spans="1:39" x14ac:dyDescent="0.25">
-      <c r="A4" s="31" t="s">
+      <c r="A4" s="28" t="s">
         <v>4</v>
       </c>
-      <c r="B4" s="31">
+      <c r="B4" s="28">
         <v>1</v>
       </c>
       <c r="C4" s="3">
@@ -858,11 +858,11 @@
       <c r="D4" s="3">
         <v>1275</v>
       </c>
-      <c r="E4" s="29">
+      <c r="E4" s="26">
         <f>SUM(D4:D5)</f>
         <v>2550</v>
       </c>
-      <c r="F4" s="21">
+      <c r="F4" s="31">
         <f>E4/$E$13</f>
         <v>0.22222222222222221</v>
       </c>
@@ -873,7 +873,7 @@
         <f>G4/$D4</f>
         <v>1</v>
       </c>
-      <c r="I4" s="23">
+      <c r="I4" s="22">
         <f>SUM(G4:G5)/$E4</f>
         <v>0.91568627450980389</v>
       </c>
@@ -884,7 +884,7 @@
         <f>J4/$D4</f>
         <v>0.37176470588235294</v>
       </c>
-      <c r="L4" s="23">
+      <c r="L4" s="22">
         <f>SUM(J4:J5)/$E4</f>
         <v>0.26588235294117646</v>
       </c>
@@ -895,7 +895,7 @@
         <f>M4/$D4</f>
         <v>1</v>
       </c>
-      <c r="O4" s="23">
+      <c r="O4" s="22">
         <f>SUM(M4:M5)/$E4</f>
         <v>1</v>
       </c>
@@ -906,7 +906,7 @@
         <f>P4/$D4</f>
         <v>1</v>
       </c>
-      <c r="R4" s="23">
+      <c r="R4" s="22">
         <f>SUM(P4:P5)/$E4</f>
         <v>0.88470588235294123</v>
       </c>
@@ -917,7 +917,7 @@
         <f>S4/$D4</f>
         <v>1</v>
       </c>
-      <c r="U4" s="23">
+      <c r="U4" s="22">
         <f>SUM(S4:S5)/$E4</f>
         <v>0.83137254901960789</v>
       </c>
@@ -928,7 +928,7 @@
         <f>V4/$D4</f>
         <v>1</v>
       </c>
-      <c r="X4" s="23">
+      <c r="X4" s="22">
         <f>SUM(V4:V5)/$E4</f>
         <v>0.97450980392156861</v>
       </c>
@@ -939,7 +939,7 @@
         <f>Y4/$D4</f>
         <v>1</v>
       </c>
-      <c r="AA4" s="23">
+      <c r="AA4" s="22">
         <f>SUM(Y4:Y5)/$E4</f>
         <v>1</v>
       </c>
@@ -950,7 +950,7 @@
         <f>AB4/$D4</f>
         <v>1</v>
       </c>
-      <c r="AD4" s="23">
+      <c r="AD4" s="22">
         <f>SUM(AB4:AB5)/$E4</f>
         <v>0.87254901960784315</v>
       </c>
@@ -961,7 +961,7 @@
         <f>AE4/$D4</f>
         <v>1</v>
       </c>
-      <c r="AG4" s="23">
+      <c r="AG4" s="22">
         <f>SUM(AE4:AE5)/$E4</f>
         <v>0.88666666666666671</v>
       </c>
@@ -972,7 +972,7 @@
         <f>AH4/$D4</f>
         <v>1</v>
       </c>
-      <c r="AJ4" s="23">
+      <c r="AJ4" s="22">
         <f>SUM(AH4:AH5)/$E4</f>
         <v>0.84352941176470586</v>
       </c>
@@ -983,22 +983,22 @@
         <f>AK4/$D4</f>
         <v>0.4180392156862745</v>
       </c>
-      <c r="AM4" s="23">
+      <c r="AM4" s="22">
         <f>SUM(AK4:AK5)/$E4</f>
         <v>0.30627450980392157</v>
       </c>
     </row>
     <row r="5" spans="1:39" x14ac:dyDescent="0.25">
-      <c r="A5" s="32"/>
-      <c r="B5" s="32"/>
+      <c r="A5" s="29"/>
+      <c r="B5" s="29"/>
       <c r="C5" s="4">
         <v>1</v>
       </c>
       <c r="D5" s="4">
         <v>1275</v>
       </c>
-      <c r="E5" s="30"/>
-      <c r="F5" s="22"/>
+      <c r="E5" s="27"/>
+      <c r="F5" s="32"/>
       <c r="G5" s="12">
         <v>1060</v>
       </c>
@@ -1006,7 +1006,7 @@
         <f t="shared" ref="H5:H12" si="0">G5/$D5</f>
         <v>0.83137254901960789</v>
       </c>
-      <c r="I5" s="24"/>
+      <c r="I5" s="23"/>
       <c r="J5" s="4">
         <v>204</v>
       </c>
@@ -1014,7 +1014,7 @@
         <f t="shared" ref="K5:K12" si="1">J5/$D5</f>
         <v>0.16</v>
       </c>
-      <c r="L5" s="24"/>
+      <c r="L5" s="23"/>
       <c r="M5" s="4">
         <v>1275</v>
       </c>
@@ -1022,7 +1022,7 @@
         <f t="shared" ref="N5:N12" si="2">M5/$D5</f>
         <v>1</v>
       </c>
-      <c r="O5" s="24"/>
+      <c r="O5" s="23"/>
       <c r="P5" s="4">
         <v>981</v>
       </c>
@@ -1030,7 +1030,7 @@
         <f t="shared" ref="Q5:Q12" si="3">P5/$D5</f>
         <v>0.76941176470588235</v>
       </c>
-      <c r="R5" s="24"/>
+      <c r="R5" s="23"/>
       <c r="S5" s="4">
         <v>845</v>
       </c>
@@ -1038,7 +1038,7 @@
         <f t="shared" ref="T5:T12" si="4">S5/$D5</f>
         <v>0.66274509803921566</v>
       </c>
-      <c r="U5" s="24"/>
+      <c r="U5" s="23"/>
       <c r="V5" s="4">
         <v>1210</v>
       </c>
@@ -1046,7 +1046,7 @@
         <f t="shared" ref="W5:W12" si="5">V5/$D5</f>
         <v>0.94901960784313721</v>
       </c>
-      <c r="X5" s="24"/>
+      <c r="X5" s="23"/>
       <c r="Y5" s="4">
         <v>1275</v>
       </c>
@@ -1054,7 +1054,7 @@
         <f t="shared" ref="Z5:Z12" si="6">Y5/$D5</f>
         <v>1</v>
       </c>
-      <c r="AA5" s="24"/>
+      <c r="AA5" s="23"/>
       <c r="AB5" s="4">
         <v>950</v>
       </c>
@@ -1062,7 +1062,7 @@
         <f t="shared" ref="AC5:AC12" si="7">AB5/$D5</f>
         <v>0.74509803921568629</v>
       </c>
-      <c r="AD5" s="24"/>
+      <c r="AD5" s="23"/>
       <c r="AE5" s="4">
         <v>986</v>
       </c>
@@ -1070,7 +1070,7 @@
         <f t="shared" ref="AF5:AF12" si="8">AE5/$D5</f>
         <v>0.77333333333333332</v>
       </c>
-      <c r="AG5" s="24"/>
+      <c r="AG5" s="23"/>
       <c r="AH5" s="4">
         <v>876</v>
       </c>
@@ -1078,7 +1078,7 @@
         <f t="shared" ref="AI5:AI12" si="9">AH5/$D5</f>
         <v>0.68705882352941172</v>
       </c>
-      <c r="AJ5" s="24"/>
+      <c r="AJ5" s="23"/>
       <c r="AK5" s="4">
         <v>248</v>
       </c>
@@ -1086,13 +1086,13 @@
         <f t="shared" ref="AL5:AL12" si="10">AK5/$D5</f>
         <v>0.19450980392156864</v>
       </c>
-      <c r="AM5" s="24"/>
+      <c r="AM5" s="23"/>
     </row>
     <row r="6" spans="1:39" x14ac:dyDescent="0.25">
-      <c r="A6" s="31" t="s">
+      <c r="A6" s="28" t="s">
         <v>5</v>
       </c>
-      <c r="B6" s="31">
+      <c r="B6" s="28">
         <v>1</v>
       </c>
       <c r="C6" s="3">
@@ -1101,11 +1101,11 @@
       <c r="D6" s="3">
         <v>1530</v>
       </c>
-      <c r="E6" s="29">
+      <c r="E6" s="26">
         <f>SUM(D6:D7)</f>
         <v>3060</v>
       </c>
-      <c r="F6" s="21">
+      <c r="F6" s="31">
         <f t="shared" ref="F6" si="11">E6/$E$13</f>
         <v>0.26666666666666666</v>
       </c>
@@ -1116,7 +1116,7 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="I6" s="23">
+      <c r="I6" s="22">
         <f t="shared" ref="I6" si="12">SUM(G6:G7)/$E6</f>
         <v>3.2679738562091501E-4</v>
       </c>
@@ -1127,7 +1127,7 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="L6" s="23">
+      <c r="L6" s="22">
         <f t="shared" ref="L6" si="13">SUM(J6:J7)/$E6</f>
         <v>0</v>
       </c>
@@ -1138,7 +1138,7 @@
         <f t="shared" si="2"/>
         <v>1</v>
       </c>
-      <c r="O6" s="23">
+      <c r="O6" s="22">
         <f t="shared" ref="O6" si="14">SUM(M6:M7)/$E6</f>
         <v>1</v>
       </c>
@@ -1149,7 +1149,7 @@
         <f t="shared" si="3"/>
         <v>1</v>
       </c>
-      <c r="R6" s="23">
+      <c r="R6" s="22">
         <f t="shared" ref="R6" si="15">SUM(P6:P7)/$E6</f>
         <v>0.9137254901960784</v>
       </c>
@@ -1160,7 +1160,7 @@
         <f t="shared" si="4"/>
         <v>1</v>
       </c>
-      <c r="U6" s="23">
+      <c r="U6" s="22">
         <f t="shared" ref="U6" si="16">SUM(S6:S7)/$E6</f>
         <v>0.88366013071895422</v>
       </c>
@@ -1171,7 +1171,7 @@
         <f t="shared" si="5"/>
         <v>1</v>
       </c>
-      <c r="X6" s="23">
+      <c r="X6" s="22">
         <f t="shared" ref="X6" si="17">SUM(V6:V7)/$E6</f>
         <v>0.98986928104575167</v>
       </c>
@@ -1182,7 +1182,7 @@
         <f t="shared" si="6"/>
         <v>1</v>
       </c>
-      <c r="AA6" s="23">
+      <c r="AA6" s="22">
         <f t="shared" ref="AA6" si="18">SUM(Y6:Y7)/$E6</f>
         <v>1</v>
       </c>
@@ -1193,7 +1193,7 @@
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
-      <c r="AD6" s="23">
+      <c r="AD6" s="22">
         <f t="shared" ref="AD6" si="19">SUM(AB6:AB7)/$E6</f>
         <v>0</v>
       </c>
@@ -1204,7 +1204,7 @@
         <f t="shared" si="8"/>
         <v>0</v>
       </c>
-      <c r="AG6" s="23">
+      <c r="AG6" s="22">
         <f t="shared" ref="AG6" si="20">SUM(AE6:AE7)/$E6</f>
         <v>0</v>
       </c>
@@ -1215,7 +1215,7 @@
         <f t="shared" si="9"/>
         <v>0</v>
       </c>
-      <c r="AJ6" s="23">
+      <c r="AJ6" s="22">
         <f t="shared" ref="AJ6" si="21">SUM(AH6:AH7)/$E6</f>
         <v>0</v>
       </c>
@@ -1226,22 +1226,22 @@
         <f t="shared" si="10"/>
         <v>6.5359477124183002E-4</v>
       </c>
-      <c r="AM6" s="23">
+      <c r="AM6" s="22">
         <f t="shared" ref="AM6" si="22">SUM(AK6:AK7)/$E6</f>
         <v>3.2679738562091501E-4</v>
       </c>
     </row>
     <row r="7" spans="1:39" x14ac:dyDescent="0.25">
-      <c r="A7" s="32"/>
-      <c r="B7" s="32"/>
+      <c r="A7" s="29"/>
+      <c r="B7" s="29"/>
       <c r="C7" s="4">
         <v>1</v>
       </c>
       <c r="D7" s="4">
         <v>1530</v>
       </c>
-      <c r="E7" s="30"/>
-      <c r="F7" s="22"/>
+      <c r="E7" s="27"/>
+      <c r="F7" s="32"/>
       <c r="G7" s="12">
         <v>1</v>
       </c>
@@ -1249,7 +1249,7 @@
         <f t="shared" si="0"/>
         <v>6.5359477124183002E-4</v>
       </c>
-      <c r="I7" s="24"/>
+      <c r="I7" s="23"/>
       <c r="J7" s="4">
         <v>0</v>
       </c>
@@ -1257,7 +1257,7 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="L7" s="24"/>
+      <c r="L7" s="23"/>
       <c r="M7" s="4">
         <v>1530</v>
       </c>
@@ -1265,7 +1265,7 @@
         <f t="shared" si="2"/>
         <v>1</v>
       </c>
-      <c r="O7" s="24"/>
+      <c r="O7" s="23"/>
       <c r="P7" s="4">
         <v>1266</v>
       </c>
@@ -1273,7 +1273,7 @@
         <f t="shared" si="3"/>
         <v>0.82745098039215681</v>
       </c>
-      <c r="R7" s="24"/>
+      <c r="R7" s="23"/>
       <c r="S7" s="4">
         <v>1174</v>
       </c>
@@ -1281,7 +1281,7 @@
         <f t="shared" si="4"/>
         <v>0.76732026143790855</v>
       </c>
-      <c r="U7" s="24"/>
+      <c r="U7" s="23"/>
       <c r="V7" s="4">
         <v>1499</v>
       </c>
@@ -1289,7 +1289,7 @@
         <f t="shared" si="5"/>
         <v>0.97973856209150323</v>
       </c>
-      <c r="X7" s="24"/>
+      <c r="X7" s="23"/>
       <c r="Y7" s="4">
         <v>1530</v>
       </c>
@@ -1297,7 +1297,7 @@
         <f t="shared" si="6"/>
         <v>1</v>
       </c>
-      <c r="AA7" s="24"/>
+      <c r="AA7" s="23"/>
       <c r="AB7" s="4">
         <v>0</v>
       </c>
@@ -1305,7 +1305,7 @@
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
-      <c r="AD7" s="24"/>
+      <c r="AD7" s="23"/>
       <c r="AE7" s="4">
         <v>0</v>
       </c>
@@ -1313,7 +1313,7 @@
         <f t="shared" si="8"/>
         <v>0</v>
       </c>
-      <c r="AG7" s="24"/>
+      <c r="AG7" s="23"/>
       <c r="AH7" s="4">
         <v>0</v>
       </c>
@@ -1321,7 +1321,7 @@
         <f t="shared" si="9"/>
         <v>0</v>
       </c>
-      <c r="AJ7" s="24"/>
+      <c r="AJ7" s="23"/>
       <c r="AK7" s="4">
         <v>0</v>
       </c>
@@ -1329,13 +1329,13 @@
         <f t="shared" si="10"/>
         <v>0</v>
       </c>
-      <c r="AM7" s="24"/>
+      <c r="AM7" s="23"/>
     </row>
     <row r="8" spans="1:39" x14ac:dyDescent="0.25">
-      <c r="A8" s="31" t="s">
+      <c r="A8" s="28" t="s">
         <v>6</v>
       </c>
-      <c r="B8" s="31">
+      <c r="B8" s="28">
         <v>1</v>
       </c>
       <c r="C8" s="3">
@@ -1344,11 +1344,11 @@
       <c r="D8" s="3">
         <v>1530</v>
       </c>
-      <c r="E8" s="29">
+      <c r="E8" s="26">
         <f>SUM(D8:D9)</f>
         <v>3060</v>
       </c>
-      <c r="F8" s="21">
+      <c r="F8" s="31">
         <f t="shared" ref="F8" si="23">E8/$E$13</f>
         <v>0.26666666666666666</v>
       </c>
@@ -1359,7 +1359,7 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="I8" s="23">
+      <c r="I8" s="22">
         <f t="shared" ref="I8" si="24">SUM(G8:G9)/$E8</f>
         <v>0</v>
       </c>
@@ -1370,7 +1370,7 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="L8" s="23">
+      <c r="L8" s="22">
         <f t="shared" ref="L8" si="25">SUM(J8:J9)/$E8</f>
         <v>0</v>
       </c>
@@ -1381,7 +1381,7 @@
         <f t="shared" si="2"/>
         <v>1</v>
       </c>
-      <c r="O8" s="23">
+      <c r="O8" s="22">
         <f t="shared" ref="O8" si="26">SUM(M8:M9)/$E8</f>
         <v>1</v>
       </c>
@@ -1392,7 +1392,7 @@
         <f t="shared" si="3"/>
         <v>1</v>
       </c>
-      <c r="R8" s="23">
+      <c r="R8" s="22">
         <f t="shared" ref="R8" si="27">SUM(P8:P9)/$E8</f>
         <v>0.93954248366013071</v>
       </c>
@@ -1403,7 +1403,7 @@
         <f t="shared" si="4"/>
         <v>1</v>
       </c>
-      <c r="U8" s="23">
+      <c r="U8" s="22">
         <f t="shared" ref="U8" si="28">SUM(S8:S9)/$E8</f>
         <v>0.90522875816993464</v>
       </c>
@@ -1414,7 +1414,7 @@
         <f t="shared" si="5"/>
         <v>1</v>
       </c>
-      <c r="X8" s="23">
+      <c r="X8" s="22">
         <f t="shared" ref="X8" si="29">SUM(V8:V9)/$E8</f>
         <v>0.99444444444444446</v>
       </c>
@@ -1425,7 +1425,7 @@
         <f t="shared" si="6"/>
         <v>1</v>
       </c>
-      <c r="AA8" s="23">
+      <c r="AA8" s="22">
         <f t="shared" ref="AA8" si="30">SUM(Y8:Y9)/$E8</f>
         <v>1</v>
       </c>
@@ -1436,7 +1436,7 @@
         <f t="shared" si="7"/>
         <v>0.33333333333333331</v>
       </c>
-      <c r="AD8" s="23">
+      <c r="AD8" s="22">
         <f t="shared" ref="AD8" si="31">SUM(AB8:AB9)/$E8</f>
         <v>0.29836601307189542</v>
       </c>
@@ -1447,7 +1447,7 @@
         <f t="shared" si="8"/>
         <v>0</v>
       </c>
-      <c r="AG8" s="23">
+      <c r="AG8" s="22">
         <f t="shared" ref="AG8" si="32">SUM(AE8:AE9)/$E8</f>
         <v>0</v>
       </c>
@@ -1458,7 +1458,7 @@
         <f t="shared" si="9"/>
         <v>0</v>
       </c>
-      <c r="AJ8" s="23">
+      <c r="AJ8" s="22">
         <f t="shared" ref="AJ8" si="33">SUM(AH8:AH9)/$E8</f>
         <v>0</v>
       </c>
@@ -1469,22 +1469,22 @@
         <f t="shared" si="10"/>
         <v>0</v>
       </c>
-      <c r="AM8" s="23">
+      <c r="AM8" s="22">
         <f t="shared" ref="AM8" si="34">SUM(AK8:AK9)/$E8</f>
         <v>0</v>
       </c>
     </row>
     <row r="9" spans="1:39" x14ac:dyDescent="0.25">
-      <c r="A9" s="32"/>
-      <c r="B9" s="32"/>
+      <c r="A9" s="29"/>
+      <c r="B9" s="29"/>
       <c r="C9" s="4">
         <v>1</v>
       </c>
       <c r="D9" s="4">
         <v>1530</v>
       </c>
-      <c r="E9" s="30"/>
-      <c r="F9" s="22"/>
+      <c r="E9" s="27"/>
+      <c r="F9" s="32"/>
       <c r="G9" s="12">
         <v>0</v>
       </c>
@@ -1492,7 +1492,7 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="I9" s="24"/>
+      <c r="I9" s="23"/>
       <c r="J9" s="4">
         <v>0</v>
       </c>
@@ -1500,7 +1500,7 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="L9" s="24"/>
+      <c r="L9" s="23"/>
       <c r="M9" s="4">
         <v>1530</v>
       </c>
@@ -1508,7 +1508,7 @@
         <f t="shared" si="2"/>
         <v>1</v>
       </c>
-      <c r="O9" s="24"/>
+      <c r="O9" s="23"/>
       <c r="P9" s="4">
         <v>1345</v>
       </c>
@@ -1516,7 +1516,7 @@
         <f t="shared" si="3"/>
         <v>0.87908496732026142</v>
       </c>
-      <c r="R9" s="24"/>
+      <c r="R9" s="23"/>
       <c r="S9" s="4">
         <v>1240</v>
       </c>
@@ -1524,7 +1524,7 @@
         <f t="shared" si="4"/>
         <v>0.81045751633986929</v>
       </c>
-      <c r="U9" s="24"/>
+      <c r="U9" s="23"/>
       <c r="V9" s="4">
         <v>1513</v>
       </c>
@@ -1532,7 +1532,7 @@
         <f t="shared" si="5"/>
         <v>0.98888888888888893</v>
       </c>
-      <c r="X9" s="24"/>
+      <c r="X9" s="23"/>
       <c r="Y9" s="4">
         <v>1530</v>
       </c>
@@ -1540,7 +1540,7 @@
         <f t="shared" si="6"/>
         <v>1</v>
       </c>
-      <c r="AA9" s="24"/>
+      <c r="AA9" s="23"/>
       <c r="AB9" s="4">
         <v>403</v>
       </c>
@@ -1548,7 +1548,7 @@
         <f t="shared" si="7"/>
         <v>0.26339869281045752</v>
       </c>
-      <c r="AD9" s="24"/>
+      <c r="AD9" s="23"/>
       <c r="AE9" s="4">
         <v>0</v>
       </c>
@@ -1556,7 +1556,7 @@
         <f t="shared" si="8"/>
         <v>0</v>
       </c>
-      <c r="AG9" s="24"/>
+      <c r="AG9" s="23"/>
       <c r="AH9" s="4">
         <v>0</v>
       </c>
@@ -1564,7 +1564,7 @@
         <f t="shared" si="9"/>
         <v>0</v>
       </c>
-      <c r="AJ9" s="24"/>
+      <c r="AJ9" s="23"/>
       <c r="AK9" s="4">
         <v>0</v>
       </c>
@@ -1572,13 +1572,13 @@
         <f t="shared" si="10"/>
         <v>0</v>
       </c>
-      <c r="AM9" s="24"/>
+      <c r="AM9" s="23"/>
     </row>
     <row r="10" spans="1:39" x14ac:dyDescent="0.25">
-      <c r="A10" s="31" t="s">
+      <c r="A10" s="28" t="s">
         <v>7</v>
       </c>
-      <c r="B10" s="31">
+      <c r="B10" s="28">
         <v>1</v>
       </c>
       <c r="C10" s="3">
@@ -1587,11 +1587,11 @@
       <c r="D10" s="3">
         <v>1275</v>
       </c>
-      <c r="E10" s="29">
+      <c r="E10" s="26">
         <f>SUM(D10:D11)</f>
         <v>2550</v>
       </c>
-      <c r="F10" s="21">
+      <c r="F10" s="31">
         <f t="shared" ref="F10" si="35">E10/$E$13</f>
         <v>0.22222222222222221</v>
       </c>
@@ -1602,7 +1602,7 @@
         <f t="shared" si="0"/>
         <v>0.76313725490196083</v>
       </c>
-      <c r="I10" s="23">
+      <c r="I10" s="22">
         <f t="shared" ref="I10" si="36">SUM(G10:G11)/$E10</f>
         <v>0.55450980392156868</v>
       </c>
@@ -1613,7 +1613,7 @@
         <f t="shared" si="1"/>
         <v>7.8431372549019607E-2</v>
       </c>
-      <c r="L10" s="23">
+      <c r="L10" s="22">
         <f t="shared" ref="L10" si="37">SUM(J10:J11)/$E10</f>
         <v>5.2156862745098037E-2</v>
       </c>
@@ -1624,7 +1624,7 @@
         <f t="shared" si="2"/>
         <v>1</v>
       </c>
-      <c r="O10" s="23">
+      <c r="O10" s="22">
         <f t="shared" ref="O10" si="38">SUM(M10:M11)/$E10</f>
         <v>1</v>
       </c>
@@ -1635,7 +1635,7 @@
         <f t="shared" si="3"/>
         <v>0.99921568627450985</v>
       </c>
-      <c r="R10" s="23">
+      <c r="R10" s="22">
         <f t="shared" ref="R10" si="39">SUM(P10:P11)/$E10</f>
         <v>0.83450980392156859</v>
       </c>
@@ -1646,7 +1646,7 @@
         <f t="shared" si="4"/>
         <v>1</v>
       </c>
-      <c r="U10" s="23">
+      <c r="U10" s="22">
         <f t="shared" ref="U10" si="40">SUM(S10:S11)/$E10</f>
         <v>0.82823529411764707</v>
       </c>
@@ -1657,7 +1657,7 @@
         <f t="shared" si="5"/>
         <v>1</v>
       </c>
-      <c r="X10" s="23">
+      <c r="X10" s="22">
         <f t="shared" ref="X10" si="41">SUM(V10:V11)/$E10</f>
         <v>0.9831372549019608</v>
       </c>
@@ -1668,7 +1668,7 @@
         <f t="shared" si="6"/>
         <v>1</v>
       </c>
-      <c r="AA10" s="23">
+      <c r="AA10" s="22">
         <f t="shared" ref="AA10" si="42">SUM(Y10:Y11)/$E10</f>
         <v>1</v>
       </c>
@@ -1679,7 +1679,7 @@
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
-      <c r="AD10" s="23">
+      <c r="AD10" s="22">
         <f t="shared" ref="AD10" si="43">SUM(AB10:AB11)/$E10</f>
         <v>0</v>
       </c>
@@ -1690,7 +1690,7 @@
         <f t="shared" si="8"/>
         <v>0.43215686274509801</v>
       </c>
-      <c r="AG10" s="23">
+      <c r="AG10" s="22">
         <f t="shared" ref="AG10" si="44">SUM(AE10:AE11)/$E10</f>
         <v>0.29058823529411765</v>
       </c>
@@ -1701,7 +1701,7 @@
         <f t="shared" si="9"/>
         <v>0.15058823529411763</v>
       </c>
-      <c r="AJ10" s="23">
+      <c r="AJ10" s="22">
         <f t="shared" ref="AJ10" si="45">SUM(AH10:AH11)/$E10</f>
         <v>9.9607843137254903E-2</v>
       </c>
@@ -1712,22 +1712,22 @@
         <f t="shared" si="10"/>
         <v>0.10901960784313726</v>
       </c>
-      <c r="AM10" s="23">
+      <c r="AM10" s="22">
         <f t="shared" ref="AM10" si="46">SUM(AK10:AK11)/$E10</f>
         <v>7.7254901960784314E-2</v>
       </c>
     </row>
     <row r="11" spans="1:39" x14ac:dyDescent="0.25">
-      <c r="A11" s="32"/>
-      <c r="B11" s="32"/>
+      <c r="A11" s="29"/>
+      <c r="B11" s="29"/>
       <c r="C11" s="4">
         <v>1</v>
       </c>
       <c r="D11" s="4">
         <v>1275</v>
       </c>
-      <c r="E11" s="30"/>
-      <c r="F11" s="22"/>
+      <c r="E11" s="27"/>
+      <c r="F11" s="32"/>
       <c r="G11" s="12">
         <v>441</v>
       </c>
@@ -1735,7 +1735,7 @@
         <f t="shared" si="0"/>
         <v>0.34588235294117647</v>
       </c>
-      <c r="I11" s="24"/>
+      <c r="I11" s="23"/>
       <c r="J11" s="4">
         <v>33</v>
       </c>
@@ -1743,7 +1743,7 @@
         <f t="shared" si="1"/>
         <v>2.5882352941176471E-2</v>
       </c>
-      <c r="L11" s="24"/>
+      <c r="L11" s="23"/>
       <c r="M11" s="4">
         <v>1275</v>
       </c>
@@ -1751,7 +1751,7 @@
         <f t="shared" si="2"/>
         <v>1</v>
       </c>
-      <c r="O11" s="24"/>
+      <c r="O11" s="23"/>
       <c r="P11" s="4">
         <v>854</v>
       </c>
@@ -1759,7 +1759,7 @@
         <f t="shared" si="3"/>
         <v>0.66980392156862745</v>
       </c>
-      <c r="R11" s="24"/>
+      <c r="R11" s="23"/>
       <c r="S11" s="4">
         <v>837</v>
       </c>
@@ -1767,7 +1767,7 @@
         <f t="shared" si="4"/>
         <v>0.65647058823529414</v>
       </c>
-      <c r="U11" s="24"/>
+      <c r="U11" s="23"/>
       <c r="V11" s="4">
         <v>1232</v>
       </c>
@@ -1775,7 +1775,7 @@
         <f t="shared" si="5"/>
         <v>0.9662745098039216</v>
       </c>
-      <c r="X11" s="24"/>
+      <c r="X11" s="23"/>
       <c r="Y11" s="4">
         <v>1275</v>
       </c>
@@ -1783,7 +1783,7 @@
         <f t="shared" si="6"/>
         <v>1</v>
       </c>
-      <c r="AA11" s="24"/>
+      <c r="AA11" s="23"/>
       <c r="AB11" s="4">
         <v>0</v>
       </c>
@@ -1791,7 +1791,7 @@
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
-      <c r="AD11" s="24"/>
+      <c r="AD11" s="23"/>
       <c r="AE11" s="4">
         <v>190</v>
       </c>
@@ -1799,7 +1799,7 @@
         <f t="shared" si="8"/>
         <v>0.14901960784313725</v>
       </c>
-      <c r="AG11" s="24"/>
+      <c r="AG11" s="23"/>
       <c r="AH11" s="4">
         <v>62</v>
       </c>
@@ -1807,7 +1807,7 @@
         <f t="shared" si="9"/>
         <v>4.8627450980392159E-2</v>
       </c>
-      <c r="AJ11" s="24"/>
+      <c r="AJ11" s="23"/>
       <c r="AK11" s="4">
         <v>58</v>
       </c>
@@ -1815,7 +1815,7 @@
         <f t="shared" si="10"/>
         <v>4.5490196078431369E-2</v>
       </c>
-      <c r="AM11" s="24"/>
+      <c r="AM11" s="23"/>
     </row>
     <row r="12" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A12" s="14" t="s">
@@ -1960,12 +1960,12 @@
       </c>
     </row>
     <row r="13" spans="1:39" x14ac:dyDescent="0.25">
-      <c r="A13" s="26" t="s">
-        <v>0</v>
-      </c>
-      <c r="B13" s="26"/>
-      <c r="C13" s="26"/>
-      <c r="D13" s="26"/>
+      <c r="A13" s="21" t="s">
+        <v>0</v>
+      </c>
+      <c r="B13" s="21"/>
+      <c r="C13" s="21"/>
+      <c r="D13" s="21"/>
       <c r="E13">
         <f>SUM(E4:E12)</f>
         <v>11475</v>
@@ -2057,7 +2057,7 @@
       </c>
       <c r="AI13" s="5"/>
       <c r="AJ13" s="5">
-        <f t="shared" ref="AJ13:AJ14" si="65">AH13/$E13</f>
+        <f t="shared" ref="AJ13" si="65">AH13/$E13</f>
         <v>0.20958605664488017</v>
       </c>
       <c r="AK13">
@@ -2177,6 +2177,63 @@
   </sheetData>
   <autoFilter ref="A3:AM3" xr:uid="{A7555910-4F01-4A83-83B1-DAA1B4FA9702}"/>
   <mergeCells count="73">
+    <mergeCell ref="F10:F11"/>
+    <mergeCell ref="F8:F9"/>
+    <mergeCell ref="F6:F7"/>
+    <mergeCell ref="F4:F5"/>
+    <mergeCell ref="AJ4:AJ5"/>
+    <mergeCell ref="AJ6:AJ7"/>
+    <mergeCell ref="AJ8:AJ9"/>
+    <mergeCell ref="AJ10:AJ11"/>
+    <mergeCell ref="X4:X5"/>
+    <mergeCell ref="X6:X7"/>
+    <mergeCell ref="X8:X9"/>
+    <mergeCell ref="X10:X11"/>
+    <mergeCell ref="AA4:AA5"/>
+    <mergeCell ref="AA6:AA7"/>
+    <mergeCell ref="AA8:AA9"/>
+    <mergeCell ref="AA10:AA11"/>
+    <mergeCell ref="AM6:AM7"/>
+    <mergeCell ref="AM8:AM9"/>
+    <mergeCell ref="AM10:AM11"/>
+    <mergeCell ref="AD4:AD5"/>
+    <mergeCell ref="AD6:AD7"/>
+    <mergeCell ref="AD8:AD9"/>
+    <mergeCell ref="AD10:AD11"/>
+    <mergeCell ref="AG4:AG5"/>
+    <mergeCell ref="AG6:AG7"/>
+    <mergeCell ref="AG8:AG9"/>
+    <mergeCell ref="AG10:AG11"/>
+    <mergeCell ref="R8:R9"/>
+    <mergeCell ref="R10:R11"/>
+    <mergeCell ref="U4:U5"/>
+    <mergeCell ref="U6:U7"/>
+    <mergeCell ref="U8:U9"/>
+    <mergeCell ref="U10:U11"/>
+    <mergeCell ref="L8:L9"/>
+    <mergeCell ref="L10:L11"/>
+    <mergeCell ref="O4:O5"/>
+    <mergeCell ref="O6:O7"/>
+    <mergeCell ref="O8:O9"/>
+    <mergeCell ref="O10:O11"/>
+    <mergeCell ref="AK2:AM2"/>
+    <mergeCell ref="AH2:AJ2"/>
+    <mergeCell ref="AE2:AG2"/>
+    <mergeCell ref="AB2:AD2"/>
+    <mergeCell ref="I4:I5"/>
+    <mergeCell ref="Y2:AA2"/>
+    <mergeCell ref="V2:X2"/>
+    <mergeCell ref="S2:U2"/>
+    <mergeCell ref="P2:R2"/>
+    <mergeCell ref="M2:O2"/>
+    <mergeCell ref="J2:L2"/>
+    <mergeCell ref="AM4:AM5"/>
+    <mergeCell ref="G2:I2"/>
+    <mergeCell ref="I6:I7"/>
+    <mergeCell ref="L4:L5"/>
+    <mergeCell ref="L6:L7"/>
+    <mergeCell ref="R4:R5"/>
+    <mergeCell ref="R6:R7"/>
     <mergeCell ref="A13:D13"/>
     <mergeCell ref="I8:I9"/>
     <mergeCell ref="I10:I11"/>
@@ -2193,63 +2250,6 @@
     <mergeCell ref="A8:A9"/>
     <mergeCell ref="A6:A7"/>
     <mergeCell ref="A4:A5"/>
-    <mergeCell ref="I6:I7"/>
-    <mergeCell ref="L4:L5"/>
-    <mergeCell ref="L6:L7"/>
-    <mergeCell ref="R4:R5"/>
-    <mergeCell ref="R6:R7"/>
-    <mergeCell ref="AK2:AM2"/>
-    <mergeCell ref="AH2:AJ2"/>
-    <mergeCell ref="AE2:AG2"/>
-    <mergeCell ref="AB2:AD2"/>
-    <mergeCell ref="I4:I5"/>
-    <mergeCell ref="Y2:AA2"/>
-    <mergeCell ref="V2:X2"/>
-    <mergeCell ref="S2:U2"/>
-    <mergeCell ref="P2:R2"/>
-    <mergeCell ref="M2:O2"/>
-    <mergeCell ref="J2:L2"/>
-    <mergeCell ref="AM4:AM5"/>
-    <mergeCell ref="G2:I2"/>
-    <mergeCell ref="L8:L9"/>
-    <mergeCell ref="L10:L11"/>
-    <mergeCell ref="O4:O5"/>
-    <mergeCell ref="O6:O7"/>
-    <mergeCell ref="O8:O9"/>
-    <mergeCell ref="O10:O11"/>
-    <mergeCell ref="R8:R9"/>
-    <mergeCell ref="R10:R11"/>
-    <mergeCell ref="U4:U5"/>
-    <mergeCell ref="U6:U7"/>
-    <mergeCell ref="U8:U9"/>
-    <mergeCell ref="U10:U11"/>
-    <mergeCell ref="AM6:AM7"/>
-    <mergeCell ref="AM8:AM9"/>
-    <mergeCell ref="AM10:AM11"/>
-    <mergeCell ref="AD4:AD5"/>
-    <mergeCell ref="AD6:AD7"/>
-    <mergeCell ref="AD8:AD9"/>
-    <mergeCell ref="AD10:AD11"/>
-    <mergeCell ref="AG4:AG5"/>
-    <mergeCell ref="AG6:AG7"/>
-    <mergeCell ref="AG8:AG9"/>
-    <mergeCell ref="AG10:AG11"/>
-    <mergeCell ref="F10:F11"/>
-    <mergeCell ref="F8:F9"/>
-    <mergeCell ref="F6:F7"/>
-    <mergeCell ref="F4:F5"/>
-    <mergeCell ref="AJ4:AJ5"/>
-    <mergeCell ref="AJ6:AJ7"/>
-    <mergeCell ref="AJ8:AJ9"/>
-    <mergeCell ref="AJ10:AJ11"/>
-    <mergeCell ref="X4:X5"/>
-    <mergeCell ref="X6:X7"/>
-    <mergeCell ref="X8:X9"/>
-    <mergeCell ref="X10:X11"/>
-    <mergeCell ref="AA4:AA5"/>
-    <mergeCell ref="AA6:AA7"/>
-    <mergeCell ref="AA8:AA9"/>
-    <mergeCell ref="AA10:AA11"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Corrected CO2 and GHG Emissions
</commit_message>
<xml_diff>
--- a/model_outputs/impacts/reductions.xlsx
+++ b/model_outputs/impacts/reductions.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://gtvault-my.sharepoint.com/personal/obroesicke3_gatech_edu/Documents/00_PhD/GitHub/DistributedEnergyGen/model_outputs/impacts/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="77" documentId="8_{D10A294E-E8C7-4A00-AE8A-00FCE5A3AFD0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{BC7B997F-5B24-4902-9DB1-900068CC9097}"/>
+  <xr:revisionPtr revIDLastSave="84" documentId="8_{D10A294E-E8C7-4A00-AE8A-00FCE5A3AFD0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{013EB87D-C509-462F-B5A5-CE4DACA75A24}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{32BF44EB-935B-4F4B-BDC1-B755049E81DC}"/>
+    <workbookView xWindow="29835" yWindow="1740" windowWidth="21600" windowHeight="11385" xr2:uid="{32BF44EB-935B-4F4B-BDC1-B755049E81DC}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -260,15 +260,24 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="2" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="2" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="9" fontId="0" fillId="2" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="2" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -286,15 +295,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -614,10 +614,10 @@
   <dimension ref="A1:AM18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="5" ySplit="3" topLeftCell="H4" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="5" ySplit="3" topLeftCell="M4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="F1" sqref="F1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="U20" sqref="U20"/>
+      <selection pane="bottomRight" activeCell="AH4" sqref="AH4:AH12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -669,64 +669,64 @@
       </c>
     </row>
     <row r="2" spans="1:39" x14ac:dyDescent="0.25">
-      <c r="F2" s="24" t="s">
+      <c r="F2" s="27" t="s">
         <v>26</v>
       </c>
-      <c r="G2" s="30" t="s">
+      <c r="G2" s="25" t="s">
         <v>10</v>
       </c>
-      <c r="H2" s="30"/>
-      <c r="I2" s="30"/>
-      <c r="J2" s="30" t="s">
+      <c r="H2" s="25"/>
+      <c r="I2" s="25"/>
+      <c r="J2" s="25" t="s">
         <v>11</v>
       </c>
-      <c r="K2" s="30"/>
-      <c r="L2" s="30"/>
-      <c r="M2" s="30" t="s">
+      <c r="K2" s="25"/>
+      <c r="L2" s="25"/>
+      <c r="M2" s="25" t="s">
         <v>12</v>
       </c>
-      <c r="N2" s="30"/>
-      <c r="O2" s="30"/>
-      <c r="P2" s="30" t="s">
+      <c r="N2" s="25"/>
+      <c r="O2" s="25"/>
+      <c r="P2" s="25" t="s">
         <v>13</v>
       </c>
-      <c r="Q2" s="30"/>
-      <c r="R2" s="30"/>
-      <c r="S2" s="30" t="s">
+      <c r="Q2" s="25"/>
+      <c r="R2" s="25"/>
+      <c r="S2" s="25" t="s">
         <v>14</v>
       </c>
-      <c r="T2" s="30"/>
-      <c r="U2" s="30"/>
-      <c r="V2" s="30" t="s">
+      <c r="T2" s="25"/>
+      <c r="U2" s="25"/>
+      <c r="V2" s="25" t="s">
         <v>15</v>
       </c>
-      <c r="W2" s="30"/>
-      <c r="X2" s="30"/>
-      <c r="Y2" s="30" t="s">
+      <c r="W2" s="25"/>
+      <c r="X2" s="25"/>
+      <c r="Y2" s="25" t="s">
         <v>16</v>
       </c>
-      <c r="Z2" s="30"/>
-      <c r="AA2" s="30"/>
-      <c r="AB2" s="30" t="s">
+      <c r="Z2" s="25"/>
+      <c r="AA2" s="25"/>
+      <c r="AB2" s="25" t="s">
         <v>17</v>
       </c>
-      <c r="AC2" s="30"/>
-      <c r="AD2" s="30"/>
-      <c r="AE2" s="30" t="s">
+      <c r="AC2" s="25"/>
+      <c r="AD2" s="25"/>
+      <c r="AE2" s="25" t="s">
         <v>18</v>
       </c>
-      <c r="AF2" s="30"/>
-      <c r="AG2" s="30"/>
-      <c r="AH2" s="30" t="s">
+      <c r="AF2" s="25"/>
+      <c r="AG2" s="25"/>
+      <c r="AH2" s="25" t="s">
         <v>19</v>
       </c>
-      <c r="AI2" s="30"/>
-      <c r="AJ2" s="30"/>
-      <c r="AK2" s="30" t="s">
+      <c r="AI2" s="25"/>
+      <c r="AJ2" s="25"/>
+      <c r="AK2" s="25" t="s">
         <v>20</v>
       </c>
-      <c r="AL2" s="30"/>
-      <c r="AM2" s="30"/>
+      <c r="AL2" s="25"/>
+      <c r="AM2" s="25"/>
     </row>
     <row r="3" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
@@ -744,7 +744,7 @@
       <c r="E3" t="s">
         <v>25</v>
       </c>
-      <c r="F3" s="25"/>
+      <c r="F3" s="28"/>
       <c r="G3" s="1" t="s">
         <v>21</v>
       </c>
@@ -846,10 +846,10 @@
       </c>
     </row>
     <row r="4" spans="1:39" x14ac:dyDescent="0.25">
-      <c r="A4" s="28" t="s">
+      <c r="A4" s="31" t="s">
         <v>4</v>
       </c>
-      <c r="B4" s="28">
+      <c r="B4" s="31">
         <v>1</v>
       </c>
       <c r="C4" s="3">
@@ -858,35 +858,35 @@
       <c r="D4" s="3">
         <v>1275</v>
       </c>
-      <c r="E4" s="26">
+      <c r="E4" s="29">
         <f>SUM(D4:D5)</f>
         <v>2550</v>
       </c>
-      <c r="F4" s="31">
+      <c r="F4" s="21">
         <f>E4/$E$13</f>
         <v>0.22222222222222221</v>
       </c>
       <c r="G4" s="10">
-        <v>1275</v>
+        <v>1140</v>
       </c>
       <c r="H4" s="11">
         <f>G4/$D4</f>
-        <v>1</v>
-      </c>
-      <c r="I4" s="22">
+        <v>0.89411764705882357</v>
+      </c>
+      <c r="I4" s="23">
         <f>SUM(G4:G5)/$E4</f>
-        <v>0.91568627450980389</v>
+        <v>0.65960784313725496</v>
       </c>
       <c r="J4" s="3">
-        <v>474</v>
+        <v>479</v>
       </c>
       <c r="K4" s="11">
         <f>J4/$D4</f>
-        <v>0.37176470588235294</v>
-      </c>
-      <c r="L4" s="22">
+        <v>0.37568627450980391</v>
+      </c>
+      <c r="L4" s="23">
         <f>SUM(J4:J5)/$E4</f>
-        <v>0.26588235294117646</v>
+        <v>0.26627450980392159</v>
       </c>
       <c r="M4" s="3">
         <v>1275</v>
@@ -895,9 +895,9 @@
         <f>M4/$D4</f>
         <v>1</v>
       </c>
-      <c r="O4" s="22">
+      <c r="O4" s="23">
         <f>SUM(M4:M5)/$E4</f>
-        <v>1</v>
+        <v>0.82509803921568625</v>
       </c>
       <c r="P4" s="3">
         <v>1275</v>
@@ -906,7 +906,7 @@
         <f>P4/$D4</f>
         <v>1</v>
       </c>
-      <c r="R4" s="22">
+      <c r="R4" s="23">
         <f>SUM(P4:P5)/$E4</f>
         <v>0.88470588235294123</v>
       </c>
@@ -917,7 +917,7 @@
         <f>S4/$D4</f>
         <v>1</v>
       </c>
-      <c r="U4" s="22">
+      <c r="U4" s="23">
         <f>SUM(S4:S5)/$E4</f>
         <v>0.83137254901960789</v>
       </c>
@@ -928,7 +928,7 @@
         <f>V4/$D4</f>
         <v>1</v>
       </c>
-      <c r="X4" s="22">
+      <c r="X4" s="23">
         <f>SUM(V4:V5)/$E4</f>
         <v>0.97450980392156861</v>
       </c>
@@ -939,7 +939,7 @@
         <f>Y4/$D4</f>
         <v>1</v>
       </c>
-      <c r="AA4" s="22">
+      <c r="AA4" s="23">
         <f>SUM(Y4:Y5)/$E4</f>
         <v>1</v>
       </c>
@@ -950,31 +950,31 @@
         <f>AB4/$D4</f>
         <v>1</v>
       </c>
-      <c r="AD4" s="22">
+      <c r="AD4" s="23">
         <f>SUM(AB4:AB5)/$E4</f>
         <v>0.87254901960784315</v>
       </c>
       <c r="AE4" s="3">
-        <v>1275</v>
+        <v>1119</v>
       </c>
       <c r="AF4" s="11">
         <f>AE4/$D4</f>
-        <v>1</v>
-      </c>
-      <c r="AG4" s="22">
+        <v>0.87764705882352945</v>
+      </c>
+      <c r="AG4" s="23">
         <f>SUM(AE4:AE5)/$E4</f>
-        <v>0.88666666666666671</v>
+        <v>0.61803921568627451</v>
       </c>
       <c r="AH4" s="3">
-        <v>1275</v>
+        <v>736</v>
       </c>
       <c r="AI4" s="11">
         <f>AH4/$D4</f>
-        <v>1</v>
-      </c>
-      <c r="AJ4" s="22">
+        <v>0.57725490196078433</v>
+      </c>
+      <c r="AJ4" s="23">
         <f>SUM(AH4:AH5)/$E4</f>
-        <v>0.84352941176470586</v>
+        <v>0.39176470588235296</v>
       </c>
       <c r="AK4" s="3">
         <v>533</v>
@@ -983,46 +983,46 @@
         <f>AK4/$D4</f>
         <v>0.4180392156862745</v>
       </c>
-      <c r="AM4" s="22">
+      <c r="AM4" s="23">
         <f>SUM(AK4:AK5)/$E4</f>
         <v>0.30627450980392157</v>
       </c>
     </row>
     <row r="5" spans="1:39" x14ac:dyDescent="0.25">
-      <c r="A5" s="29"/>
-      <c r="B5" s="29"/>
+      <c r="A5" s="32"/>
+      <c r="B5" s="32"/>
       <c r="C5" s="4">
         <v>1</v>
       </c>
       <c r="D5" s="4">
         <v>1275</v>
       </c>
-      <c r="E5" s="27"/>
-      <c r="F5" s="32"/>
+      <c r="E5" s="30"/>
+      <c r="F5" s="22"/>
       <c r="G5" s="12">
-        <v>1060</v>
+        <v>542</v>
       </c>
       <c r="H5" s="13">
         <f t="shared" ref="H5:H12" si="0">G5/$D5</f>
-        <v>0.83137254901960789</v>
-      </c>
-      <c r="I5" s="23"/>
+        <v>0.42509803921568629</v>
+      </c>
+      <c r="I5" s="24"/>
       <c r="J5" s="4">
-        <v>204</v>
+        <v>200</v>
       </c>
       <c r="K5" s="13">
         <f t="shared" ref="K5:K12" si="1">J5/$D5</f>
-        <v>0.16</v>
-      </c>
-      <c r="L5" s="23"/>
+        <v>0.15686274509803921</v>
+      </c>
+      <c r="L5" s="24"/>
       <c r="M5" s="4">
-        <v>1275</v>
+        <v>829</v>
       </c>
       <c r="N5" s="13">
         <f t="shared" ref="N5:N12" si="2">M5/$D5</f>
-        <v>1</v>
-      </c>
-      <c r="O5" s="23"/>
+        <v>0.6501960784313725</v>
+      </c>
+      <c r="O5" s="24"/>
       <c r="P5" s="4">
         <v>981</v>
       </c>
@@ -1030,7 +1030,7 @@
         <f t="shared" ref="Q5:Q12" si="3">P5/$D5</f>
         <v>0.76941176470588235</v>
       </c>
-      <c r="R5" s="23"/>
+      <c r="R5" s="24"/>
       <c r="S5" s="4">
         <v>845</v>
       </c>
@@ -1038,7 +1038,7 @@
         <f t="shared" ref="T5:T12" si="4">S5/$D5</f>
         <v>0.66274509803921566</v>
       </c>
-      <c r="U5" s="23"/>
+      <c r="U5" s="24"/>
       <c r="V5" s="4">
         <v>1210</v>
       </c>
@@ -1046,7 +1046,7 @@
         <f t="shared" ref="W5:W12" si="5">V5/$D5</f>
         <v>0.94901960784313721</v>
       </c>
-      <c r="X5" s="23"/>
+      <c r="X5" s="24"/>
       <c r="Y5" s="4">
         <v>1275</v>
       </c>
@@ -1054,7 +1054,7 @@
         <f t="shared" ref="Z5:Z12" si="6">Y5/$D5</f>
         <v>1</v>
       </c>
-      <c r="AA5" s="23"/>
+      <c r="AA5" s="24"/>
       <c r="AB5" s="4">
         <v>950</v>
       </c>
@@ -1062,23 +1062,23 @@
         <f t="shared" ref="AC5:AC12" si="7">AB5/$D5</f>
         <v>0.74509803921568629</v>
       </c>
-      <c r="AD5" s="23"/>
+      <c r="AD5" s="24"/>
       <c r="AE5" s="4">
-        <v>986</v>
+        <v>457</v>
       </c>
       <c r="AF5" s="13">
         <f t="shared" ref="AF5:AF12" si="8">AE5/$D5</f>
-        <v>0.77333333333333332</v>
-      </c>
-      <c r="AG5" s="23"/>
+        <v>0.35843137254901963</v>
+      </c>
+      <c r="AG5" s="24"/>
       <c r="AH5" s="4">
-        <v>876</v>
+        <v>263</v>
       </c>
       <c r="AI5" s="13">
         <f t="shared" ref="AI5:AI12" si="9">AH5/$D5</f>
-        <v>0.68705882352941172</v>
-      </c>
-      <c r="AJ5" s="23"/>
+        <v>0.20627450980392156</v>
+      </c>
+      <c r="AJ5" s="24"/>
       <c r="AK5" s="4">
         <v>248</v>
       </c>
@@ -1086,13 +1086,13 @@
         <f t="shared" ref="AL5:AL12" si="10">AK5/$D5</f>
         <v>0.19450980392156864</v>
       </c>
-      <c r="AM5" s="23"/>
+      <c r="AM5" s="24"/>
     </row>
     <row r="6" spans="1:39" x14ac:dyDescent="0.25">
-      <c r="A6" s="28" t="s">
+      <c r="A6" s="31" t="s">
         <v>5</v>
       </c>
-      <c r="B6" s="28">
+      <c r="B6" s="31">
         <v>1</v>
       </c>
       <c r="C6" s="3">
@@ -1101,11 +1101,11 @@
       <c r="D6" s="3">
         <v>1530</v>
       </c>
-      <c r="E6" s="26">
+      <c r="E6" s="29">
         <f>SUM(D6:D7)</f>
         <v>3060</v>
       </c>
-      <c r="F6" s="31">
+      <c r="F6" s="21">
         <f t="shared" ref="F6" si="11">E6/$E$13</f>
         <v>0.26666666666666666</v>
       </c>
@@ -1116,9 +1116,9 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="I6" s="22">
+      <c r="I6" s="23">
         <f t="shared" ref="I6" si="12">SUM(G6:G7)/$E6</f>
-        <v>3.2679738562091501E-4</v>
+        <v>3.2679738562091504E-3</v>
       </c>
       <c r="J6" s="3">
         <v>0</v>
@@ -1127,7 +1127,7 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="L6" s="22">
+      <c r="L6" s="23">
         <f t="shared" ref="L6" si="13">SUM(J6:J7)/$E6</f>
         <v>0</v>
       </c>
@@ -1138,9 +1138,9 @@
         <f t="shared" si="2"/>
         <v>1</v>
       </c>
-      <c r="O6" s="22">
+      <c r="O6" s="23">
         <f t="shared" ref="O6" si="14">SUM(M6:M7)/$E6</f>
-        <v>1</v>
+        <v>0.8879084967320261</v>
       </c>
       <c r="P6" s="3">
         <v>1530</v>
@@ -1149,7 +1149,7 @@
         <f t="shared" si="3"/>
         <v>1</v>
       </c>
-      <c r="R6" s="22">
+      <c r="R6" s="23">
         <f t="shared" ref="R6" si="15">SUM(P6:P7)/$E6</f>
         <v>0.9137254901960784</v>
       </c>
@@ -1160,7 +1160,7 @@
         <f t="shared" si="4"/>
         <v>1</v>
       </c>
-      <c r="U6" s="22">
+      <c r="U6" s="23">
         <f t="shared" ref="U6" si="16">SUM(S6:S7)/$E6</f>
         <v>0.88366013071895422</v>
       </c>
@@ -1171,7 +1171,7 @@
         <f t="shared" si="5"/>
         <v>1</v>
       </c>
-      <c r="X6" s="22">
+      <c r="X6" s="23">
         <f t="shared" ref="X6" si="17">SUM(V6:V7)/$E6</f>
         <v>0.98986928104575167</v>
       </c>
@@ -1182,7 +1182,7 @@
         <f t="shared" si="6"/>
         <v>1</v>
       </c>
-      <c r="AA6" s="22">
+      <c r="AA6" s="23">
         <f t="shared" ref="AA6" si="18">SUM(Y6:Y7)/$E6</f>
         <v>1</v>
       </c>
@@ -1193,7 +1193,7 @@
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
-      <c r="AD6" s="22">
+      <c r="AD6" s="23">
         <f t="shared" ref="AD6" si="19">SUM(AB6:AB7)/$E6</f>
         <v>0</v>
       </c>
@@ -1204,7 +1204,7 @@
         <f t="shared" si="8"/>
         <v>0</v>
       </c>
-      <c r="AG6" s="22">
+      <c r="AG6" s="23">
         <f t="shared" ref="AG6" si="20">SUM(AE6:AE7)/$E6</f>
         <v>0</v>
       </c>
@@ -1215,7 +1215,7 @@
         <f t="shared" si="9"/>
         <v>0</v>
       </c>
-      <c r="AJ6" s="22">
+      <c r="AJ6" s="23">
         <f t="shared" ref="AJ6" si="21">SUM(AH6:AH7)/$E6</f>
         <v>0</v>
       </c>
@@ -1226,30 +1226,30 @@
         <f t="shared" si="10"/>
         <v>6.5359477124183002E-4</v>
       </c>
-      <c r="AM6" s="22">
+      <c r="AM6" s="23">
         <f t="shared" ref="AM6" si="22">SUM(AK6:AK7)/$E6</f>
         <v>3.2679738562091501E-4</v>
       </c>
     </row>
     <row r="7" spans="1:39" x14ac:dyDescent="0.25">
-      <c r="A7" s="29"/>
-      <c r="B7" s="29"/>
+      <c r="A7" s="32"/>
+      <c r="B7" s="32"/>
       <c r="C7" s="4">
         <v>1</v>
       </c>
       <c r="D7" s="4">
         <v>1530</v>
       </c>
-      <c r="E7" s="27"/>
-      <c r="F7" s="32"/>
+      <c r="E7" s="30"/>
+      <c r="F7" s="22"/>
       <c r="G7" s="12">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="H7" s="13">
         <f t="shared" si="0"/>
-        <v>6.5359477124183002E-4</v>
-      </c>
-      <c r="I7" s="23"/>
+        <v>6.5359477124183009E-3</v>
+      </c>
+      <c r="I7" s="24"/>
       <c r="J7" s="4">
         <v>0</v>
       </c>
@@ -1257,15 +1257,15 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="L7" s="23"/>
+      <c r="L7" s="24"/>
       <c r="M7" s="4">
-        <v>1530</v>
+        <v>1187</v>
       </c>
       <c r="N7" s="13">
         <f t="shared" si="2"/>
-        <v>1</v>
-      </c>
-      <c r="O7" s="23"/>
+        <v>0.77581699346405231</v>
+      </c>
+      <c r="O7" s="24"/>
       <c r="P7" s="4">
         <v>1266</v>
       </c>
@@ -1273,7 +1273,7 @@
         <f t="shared" si="3"/>
         <v>0.82745098039215681</v>
       </c>
-      <c r="R7" s="23"/>
+      <c r="R7" s="24"/>
       <c r="S7" s="4">
         <v>1174</v>
       </c>
@@ -1281,7 +1281,7 @@
         <f t="shared" si="4"/>
         <v>0.76732026143790855</v>
       </c>
-      <c r="U7" s="23"/>
+      <c r="U7" s="24"/>
       <c r="V7" s="4">
         <v>1499</v>
       </c>
@@ -1289,7 +1289,7 @@
         <f t="shared" si="5"/>
         <v>0.97973856209150323</v>
       </c>
-      <c r="X7" s="23"/>
+      <c r="X7" s="24"/>
       <c r="Y7" s="4">
         <v>1530</v>
       </c>
@@ -1297,7 +1297,7 @@
         <f t="shared" si="6"/>
         <v>1</v>
       </c>
-      <c r="AA7" s="23"/>
+      <c r="AA7" s="24"/>
       <c r="AB7" s="4">
         <v>0</v>
       </c>
@@ -1305,7 +1305,7 @@
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
-      <c r="AD7" s="23"/>
+      <c r="AD7" s="24"/>
       <c r="AE7" s="4">
         <v>0</v>
       </c>
@@ -1313,7 +1313,7 @@
         <f t="shared" si="8"/>
         <v>0</v>
       </c>
-      <c r="AG7" s="23"/>
+      <c r="AG7" s="24"/>
       <c r="AH7" s="4">
         <v>0</v>
       </c>
@@ -1321,7 +1321,7 @@
         <f t="shared" si="9"/>
         <v>0</v>
       </c>
-      <c r="AJ7" s="23"/>
+      <c r="AJ7" s="24"/>
       <c r="AK7" s="4">
         <v>0</v>
       </c>
@@ -1329,13 +1329,13 @@
         <f t="shared" si="10"/>
         <v>0</v>
       </c>
-      <c r="AM7" s="23"/>
+      <c r="AM7" s="24"/>
     </row>
     <row r="8" spans="1:39" x14ac:dyDescent="0.25">
-      <c r="A8" s="28" t="s">
+      <c r="A8" s="31" t="s">
         <v>6</v>
       </c>
-      <c r="B8" s="28">
+      <c r="B8" s="31">
         <v>1</v>
       </c>
       <c r="C8" s="3">
@@ -1344,11 +1344,11 @@
       <c r="D8" s="3">
         <v>1530</v>
       </c>
-      <c r="E8" s="26">
+      <c r="E8" s="29">
         <f>SUM(D8:D9)</f>
         <v>3060</v>
       </c>
-      <c r="F8" s="31">
+      <c r="F8" s="21">
         <f t="shared" ref="F8" si="23">E8/$E$13</f>
         <v>0.26666666666666666</v>
       </c>
@@ -1359,9 +1359,9 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="I8" s="22">
+      <c r="I8" s="23">
         <f t="shared" ref="I8" si="24">SUM(G8:G9)/$E8</f>
-        <v>0</v>
+        <v>3.2679738562091501E-4</v>
       </c>
       <c r="J8" s="3">
         <v>0</v>
@@ -1370,7 +1370,7 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="L8" s="22">
+      <c r="L8" s="23">
         <f t="shared" ref="L8" si="25">SUM(J8:J9)/$E8</f>
         <v>0</v>
       </c>
@@ -1381,9 +1381,9 @@
         <f t="shared" si="2"/>
         <v>1</v>
       </c>
-      <c r="O8" s="22">
+      <c r="O8" s="23">
         <f t="shared" ref="O8" si="26">SUM(M8:M9)/$E8</f>
-        <v>1</v>
+        <v>0.91503267973856206</v>
       </c>
       <c r="P8" s="3">
         <v>1530</v>
@@ -1392,7 +1392,7 @@
         <f t="shared" si="3"/>
         <v>1</v>
       </c>
-      <c r="R8" s="22">
+      <c r="R8" s="23">
         <f t="shared" ref="R8" si="27">SUM(P8:P9)/$E8</f>
         <v>0.93954248366013071</v>
       </c>
@@ -1403,7 +1403,7 @@
         <f t="shared" si="4"/>
         <v>1</v>
       </c>
-      <c r="U8" s="22">
+      <c r="U8" s="23">
         <f t="shared" ref="U8" si="28">SUM(S8:S9)/$E8</f>
         <v>0.90522875816993464</v>
       </c>
@@ -1414,7 +1414,7 @@
         <f t="shared" si="5"/>
         <v>1</v>
       </c>
-      <c r="X8" s="22">
+      <c r="X8" s="23">
         <f t="shared" ref="X8" si="29">SUM(V8:V9)/$E8</f>
         <v>0.99444444444444446</v>
       </c>
@@ -1425,7 +1425,7 @@
         <f t="shared" si="6"/>
         <v>1</v>
       </c>
-      <c r="AA8" s="22">
+      <c r="AA8" s="23">
         <f t="shared" ref="AA8" si="30">SUM(Y8:Y9)/$E8</f>
         <v>1</v>
       </c>
@@ -1436,7 +1436,7 @@
         <f t="shared" si="7"/>
         <v>0.33333333333333331</v>
       </c>
-      <c r="AD8" s="22">
+      <c r="AD8" s="23">
         <f t="shared" ref="AD8" si="31">SUM(AB8:AB9)/$E8</f>
         <v>0.29836601307189542</v>
       </c>
@@ -1447,7 +1447,7 @@
         <f t="shared" si="8"/>
         <v>0</v>
       </c>
-      <c r="AG8" s="22">
+      <c r="AG8" s="23">
         <f t="shared" ref="AG8" si="32">SUM(AE8:AE9)/$E8</f>
         <v>0</v>
       </c>
@@ -1458,7 +1458,7 @@
         <f t="shared" si="9"/>
         <v>0</v>
       </c>
-      <c r="AJ8" s="22">
+      <c r="AJ8" s="23">
         <f t="shared" ref="AJ8" si="33">SUM(AH8:AH9)/$E8</f>
         <v>0</v>
       </c>
@@ -1469,30 +1469,30 @@
         <f t="shared" si="10"/>
         <v>0</v>
       </c>
-      <c r="AM8" s="22">
+      <c r="AM8" s="23">
         <f t="shared" ref="AM8" si="34">SUM(AK8:AK9)/$E8</f>
         <v>0</v>
       </c>
     </row>
     <row r="9" spans="1:39" x14ac:dyDescent="0.25">
-      <c r="A9" s="29"/>
-      <c r="B9" s="29"/>
+      <c r="A9" s="32"/>
+      <c r="B9" s="32"/>
       <c r="C9" s="4">
         <v>1</v>
       </c>
       <c r="D9" s="4">
         <v>1530</v>
       </c>
-      <c r="E9" s="27"/>
-      <c r="F9" s="32"/>
+      <c r="E9" s="30"/>
+      <c r="F9" s="22"/>
       <c r="G9" s="12">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H9" s="13">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="I9" s="23"/>
+        <v>6.5359477124183002E-4</v>
+      </c>
+      <c r="I9" s="24"/>
       <c r="J9" s="4">
         <v>0</v>
       </c>
@@ -1500,15 +1500,15 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="L9" s="23"/>
+      <c r="L9" s="24"/>
       <c r="M9" s="4">
-        <v>1530</v>
+        <v>1270</v>
       </c>
       <c r="N9" s="13">
         <f t="shared" si="2"/>
-        <v>1</v>
-      </c>
-      <c r="O9" s="23"/>
+        <v>0.83006535947712423</v>
+      </c>
+      <c r="O9" s="24"/>
       <c r="P9" s="4">
         <v>1345</v>
       </c>
@@ -1516,7 +1516,7 @@
         <f t="shared" si="3"/>
         <v>0.87908496732026142</v>
       </c>
-      <c r="R9" s="23"/>
+      <c r="R9" s="24"/>
       <c r="S9" s="4">
         <v>1240</v>
       </c>
@@ -1524,7 +1524,7 @@
         <f t="shared" si="4"/>
         <v>0.81045751633986929</v>
       </c>
-      <c r="U9" s="23"/>
+      <c r="U9" s="24"/>
       <c r="V9" s="4">
         <v>1513</v>
       </c>
@@ -1532,7 +1532,7 @@
         <f t="shared" si="5"/>
         <v>0.98888888888888893</v>
       </c>
-      <c r="X9" s="23"/>
+      <c r="X9" s="24"/>
       <c r="Y9" s="4">
         <v>1530</v>
       </c>
@@ -1540,7 +1540,7 @@
         <f t="shared" si="6"/>
         <v>1</v>
       </c>
-      <c r="AA9" s="23"/>
+      <c r="AA9" s="24"/>
       <c r="AB9" s="4">
         <v>403</v>
       </c>
@@ -1548,7 +1548,7 @@
         <f t="shared" si="7"/>
         <v>0.26339869281045752</v>
       </c>
-      <c r="AD9" s="23"/>
+      <c r="AD9" s="24"/>
       <c r="AE9" s="4">
         <v>0</v>
       </c>
@@ -1556,7 +1556,7 @@
         <f t="shared" si="8"/>
         <v>0</v>
       </c>
-      <c r="AG9" s="23"/>
+      <c r="AG9" s="24"/>
       <c r="AH9" s="4">
         <v>0</v>
       </c>
@@ -1564,7 +1564,7 @@
         <f t="shared" si="9"/>
         <v>0</v>
       </c>
-      <c r="AJ9" s="23"/>
+      <c r="AJ9" s="24"/>
       <c r="AK9" s="4">
         <v>0</v>
       </c>
@@ -1572,13 +1572,13 @@
         <f t="shared" si="10"/>
         <v>0</v>
       </c>
-      <c r="AM9" s="23"/>
+      <c r="AM9" s="24"/>
     </row>
     <row r="10" spans="1:39" x14ac:dyDescent="0.25">
-      <c r="A10" s="28" t="s">
+      <c r="A10" s="31" t="s">
         <v>7</v>
       </c>
-      <c r="B10" s="28">
+      <c r="B10" s="31">
         <v>1</v>
       </c>
       <c r="C10" s="3">
@@ -1587,24 +1587,24 @@
       <c r="D10" s="3">
         <v>1275</v>
       </c>
-      <c r="E10" s="26">
+      <c r="E10" s="29">
         <f>SUM(D10:D11)</f>
         <v>2550</v>
       </c>
-      <c r="F10" s="31">
+      <c r="F10" s="21">
         <f t="shared" ref="F10" si="35">E10/$E$13</f>
         <v>0.22222222222222221</v>
       </c>
       <c r="G10" s="10">
-        <v>973</v>
+        <v>1047</v>
       </c>
       <c r="H10" s="11">
         <f t="shared" si="0"/>
-        <v>0.76313725490196083</v>
-      </c>
-      <c r="I10" s="22">
+        <v>0.82117647058823529</v>
+      </c>
+      <c r="I10" s="23">
         <f t="shared" ref="I10" si="36">SUM(G10:G11)/$E10</f>
-        <v>0.55450980392156868</v>
+        <v>0.60196078431372546</v>
       </c>
       <c r="J10" s="3">
         <v>100</v>
@@ -1613,9 +1613,9 @@
         <f t="shared" si="1"/>
         <v>7.8431372549019607E-2</v>
       </c>
-      <c r="L10" s="22">
+      <c r="L10" s="23">
         <f t="shared" ref="L10" si="37">SUM(J10:J11)/$E10</f>
-        <v>5.2156862745098037E-2</v>
+        <v>5.1372549019607847E-2</v>
       </c>
       <c r="M10" s="3">
         <v>1275</v>
@@ -1624,9 +1624,9 @@
         <f t="shared" si="2"/>
         <v>1</v>
       </c>
-      <c r="O10" s="22">
+      <c r="O10" s="23">
         <f t="shared" ref="O10" si="38">SUM(M10:M11)/$E10</f>
-        <v>1</v>
+        <v>0.8631372549019608</v>
       </c>
       <c r="P10" s="3">
         <v>1274</v>
@@ -1635,7 +1635,7 @@
         <f t="shared" si="3"/>
         <v>0.99921568627450985</v>
       </c>
-      <c r="R10" s="22">
+      <c r="R10" s="23">
         <f t="shared" ref="R10" si="39">SUM(P10:P11)/$E10</f>
         <v>0.83450980392156859</v>
       </c>
@@ -1646,7 +1646,7 @@
         <f t="shared" si="4"/>
         <v>1</v>
       </c>
-      <c r="U10" s="22">
+      <c r="U10" s="23">
         <f t="shared" ref="U10" si="40">SUM(S10:S11)/$E10</f>
         <v>0.82823529411764707</v>
       </c>
@@ -1657,7 +1657,7 @@
         <f t="shared" si="5"/>
         <v>1</v>
       </c>
-      <c r="X10" s="22">
+      <c r="X10" s="23">
         <f t="shared" ref="X10" si="41">SUM(V10:V11)/$E10</f>
         <v>0.9831372549019608</v>
       </c>
@@ -1668,7 +1668,7 @@
         <f t="shared" si="6"/>
         <v>1</v>
       </c>
-      <c r="AA10" s="22">
+      <c r="AA10" s="23">
         <f t="shared" ref="AA10" si="42">SUM(Y10:Y11)/$E10</f>
         <v>1</v>
       </c>
@@ -1679,31 +1679,31 @@
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
-      <c r="AD10" s="22">
+      <c r="AD10" s="23">
         <f t="shared" ref="AD10" si="43">SUM(AB10:AB11)/$E10</f>
         <v>0</v>
       </c>
       <c r="AE10" s="3">
-        <v>551</v>
+        <v>666</v>
       </c>
       <c r="AF10" s="11">
         <f t="shared" si="8"/>
-        <v>0.43215686274509801</v>
-      </c>
-      <c r="AG10" s="22">
+        <v>0.52235294117647058</v>
+      </c>
+      <c r="AG10" s="23">
         <f t="shared" ref="AG10" si="44">SUM(AE10:AE11)/$E10</f>
-        <v>0.29058823529411765</v>
+        <v>0.3623529411764706</v>
       </c>
       <c r="AH10" s="3">
-        <v>192</v>
+        <v>240</v>
       </c>
       <c r="AI10" s="11">
         <f t="shared" si="9"/>
-        <v>0.15058823529411763</v>
-      </c>
-      <c r="AJ10" s="22">
+        <v>0.18823529411764706</v>
+      </c>
+      <c r="AJ10" s="23">
         <f t="shared" ref="AJ10" si="45">SUM(AH10:AH11)/$E10</f>
-        <v>9.9607843137254903E-2</v>
+        <v>0.12470588235294118</v>
       </c>
       <c r="AK10" s="3">
         <v>139</v>
@@ -1712,46 +1712,46 @@
         <f t="shared" si="10"/>
         <v>0.10901960784313726</v>
       </c>
-      <c r="AM10" s="22">
+      <c r="AM10" s="23">
         <f t="shared" ref="AM10" si="46">SUM(AK10:AK11)/$E10</f>
         <v>7.7254901960784314E-2</v>
       </c>
     </row>
     <row r="11" spans="1:39" x14ac:dyDescent="0.25">
-      <c r="A11" s="29"/>
-      <c r="B11" s="29"/>
+      <c r="A11" s="32"/>
+      <c r="B11" s="32"/>
       <c r="C11" s="4">
         <v>1</v>
       </c>
       <c r="D11" s="4">
         <v>1275</v>
       </c>
-      <c r="E11" s="27"/>
-      <c r="F11" s="32"/>
+      <c r="E11" s="30"/>
+      <c r="F11" s="22"/>
       <c r="G11" s="12">
-        <v>441</v>
+        <v>488</v>
       </c>
       <c r="H11" s="13">
         <f t="shared" si="0"/>
-        <v>0.34588235294117647</v>
-      </c>
-      <c r="I11" s="23"/>
+        <v>0.38274509803921569</v>
+      </c>
+      <c r="I11" s="24"/>
       <c r="J11" s="4">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="K11" s="13">
         <f t="shared" si="1"/>
-        <v>2.5882352941176471E-2</v>
-      </c>
-      <c r="L11" s="23"/>
+        <v>2.4313725490196079E-2</v>
+      </c>
+      <c r="L11" s="24"/>
       <c r="M11" s="4">
-        <v>1275</v>
+        <v>926</v>
       </c>
       <c r="N11" s="13">
         <f t="shared" si="2"/>
-        <v>1</v>
-      </c>
-      <c r="O11" s="23"/>
+        <v>0.72627450980392161</v>
+      </c>
+      <c r="O11" s="24"/>
       <c r="P11" s="4">
         <v>854</v>
       </c>
@@ -1759,7 +1759,7 @@
         <f t="shared" si="3"/>
         <v>0.66980392156862745</v>
       </c>
-      <c r="R11" s="23"/>
+      <c r="R11" s="24"/>
       <c r="S11" s="4">
         <v>837</v>
       </c>
@@ -1767,7 +1767,7 @@
         <f t="shared" si="4"/>
         <v>0.65647058823529414</v>
       </c>
-      <c r="U11" s="23"/>
+      <c r="U11" s="24"/>
       <c r="V11" s="4">
         <v>1232</v>
       </c>
@@ -1775,7 +1775,7 @@
         <f t="shared" si="5"/>
         <v>0.9662745098039216</v>
       </c>
-      <c r="X11" s="23"/>
+      <c r="X11" s="24"/>
       <c r="Y11" s="4">
         <v>1275</v>
       </c>
@@ -1783,7 +1783,7 @@
         <f t="shared" si="6"/>
         <v>1</v>
       </c>
-      <c r="AA11" s="23"/>
+      <c r="AA11" s="24"/>
       <c r="AB11" s="4">
         <v>0</v>
       </c>
@@ -1791,23 +1791,23 @@
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
-      <c r="AD11" s="23"/>
+      <c r="AD11" s="24"/>
       <c r="AE11" s="4">
-        <v>190</v>
+        <v>258</v>
       </c>
       <c r="AF11" s="13">
         <f t="shared" si="8"/>
-        <v>0.14901960784313725</v>
-      </c>
-      <c r="AG11" s="23"/>
+        <v>0.2023529411764706</v>
+      </c>
+      <c r="AG11" s="24"/>
       <c r="AH11" s="4">
-        <v>62</v>
+        <v>78</v>
       </c>
       <c r="AI11" s="13">
         <f t="shared" si="9"/>
-        <v>4.8627450980392159E-2</v>
-      </c>
-      <c r="AJ11" s="23"/>
+        <v>6.1176470588235297E-2</v>
+      </c>
+      <c r="AJ11" s="24"/>
       <c r="AK11" s="4">
         <v>58</v>
       </c>
@@ -1815,7 +1815,7 @@
         <f t="shared" si="10"/>
         <v>4.5490196078431369E-2</v>
       </c>
-      <c r="AM11" s="23"/>
+      <c r="AM11" s="24"/>
     </row>
     <row r="12" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A12" s="14" t="s">
@@ -1860,15 +1860,15 @@
         <v>0</v>
       </c>
       <c r="M12" s="16">
-        <v>255</v>
+        <v>0</v>
       </c>
       <c r="N12" s="11">
         <f t="shared" si="2"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="O12" s="18">
         <f>M12/$E12</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="P12" s="16">
         <v>0</v>
@@ -1960,42 +1960,42 @@
       </c>
     </row>
     <row r="13" spans="1:39" x14ac:dyDescent="0.25">
-      <c r="A13" s="21" t="s">
-        <v>0</v>
-      </c>
-      <c r="B13" s="21"/>
-      <c r="C13" s="21"/>
-      <c r="D13" s="21"/>
+      <c r="A13" s="26" t="s">
+        <v>0</v>
+      </c>
+      <c r="B13" s="26"/>
+      <c r="C13" s="26"/>
+      <c r="D13" s="26"/>
       <c r="E13">
         <f>SUM(E4:E12)</f>
         <v>11475</v>
       </c>
       <c r="G13" s="9">
         <f>SUM(G4:G12)</f>
-        <v>3750</v>
+        <v>3228</v>
       </c>
       <c r="H13" s="6"/>
       <c r="I13" s="6">
         <f t="shared" ref="I13" si="47">G13/$E13</f>
-        <v>0.32679738562091504</v>
+        <v>0.28130718954248368</v>
       </c>
       <c r="J13">
         <f t="shared" ref="J13" si="48">SUM(J4:J12)</f>
-        <v>811</v>
+        <v>810</v>
       </c>
       <c r="K13" s="5"/>
       <c r="L13" s="5">
         <f t="shared" ref="L13" si="49">J13/$E13</f>
-        <v>7.0675381263616555E-2</v>
+        <v>7.0588235294117646E-2</v>
       </c>
       <c r="M13">
         <f t="shared" ref="M13" si="50">SUM(M4:M12)</f>
-        <v>11475</v>
+        <v>9822</v>
       </c>
       <c r="N13" s="5"/>
       <c r="O13" s="5">
         <f t="shared" ref="O13" si="51">M13/$E13</f>
-        <v>1</v>
+        <v>0.8559477124183007</v>
       </c>
       <c r="P13">
         <f t="shared" ref="P13" si="52">SUM(P4:P12)</f>
@@ -2044,21 +2044,21 @@
       </c>
       <c r="AE13">
         <f t="shared" ref="AE13" si="62">SUM(AE4:AE12)</f>
-        <v>3002</v>
+        <v>2500</v>
       </c>
       <c r="AF13" s="5"/>
       <c r="AG13" s="5">
         <f t="shared" ref="AG13" si="63">AE13/$E13</f>
-        <v>0.26161220043572986</v>
+        <v>0.2178649237472767</v>
       </c>
       <c r="AH13">
         <f t="shared" ref="AH13" si="64">SUM(AH4:AH12)</f>
-        <v>2405</v>
+        <v>1317</v>
       </c>
       <c r="AI13" s="5"/>
       <c r="AJ13" s="5">
         <f t="shared" ref="AJ13" si="65">AH13/$E13</f>
-        <v>0.20958605664488017</v>
+        <v>0.11477124183006536</v>
       </c>
       <c r="AK13">
         <f t="shared" ref="AK13" si="66">SUM(AK4:AK12)</f>
@@ -2093,19 +2093,19 @@
       </c>
       <c r="AE14">
         <f>SUM(AE4,AE6,AE8,AE10)</f>
-        <v>1826</v>
+        <v>1785</v>
       </c>
       <c r="AG14" s="20">
         <f>AE14/$D$14</f>
-        <v>0.32549019607843138</v>
+        <v>0.31818181818181818</v>
       </c>
       <c r="AH14">
         <f>SUM(AH4,AH6,AH8,AH10)</f>
-        <v>1467</v>
+        <v>976</v>
       </c>
       <c r="AJ14" s="20">
         <f>AH14/$D$14</f>
-        <v>0.26149732620320854</v>
+        <v>0.17397504456327986</v>
       </c>
       <c r="AK14">
         <f>SUM(AK4,AK6,AK8,AK10)</f>
@@ -2139,19 +2139,19 @@
       </c>
       <c r="AE15">
         <f>SUM(AE5,AE7,AE9,AE11)</f>
-        <v>1176</v>
+        <v>715</v>
       </c>
       <c r="AG15" s="20">
         <f>AE15/$D$14</f>
-        <v>0.20962566844919786</v>
+        <v>0.12745098039215685</v>
       </c>
       <c r="AH15">
         <f>SUM(AH5,AH7,AH9,AH11)</f>
-        <v>938</v>
+        <v>341</v>
       </c>
       <c r="AJ15" s="20">
         <f>AH15/$D$14</f>
-        <v>0.16720142602495544</v>
+        <v>6.0784313725490195E-2</v>
       </c>
       <c r="AK15">
         <f>SUM(AK5,AK7,AK9,AK11)</f>
@@ -2177,6 +2177,63 @@
   </sheetData>
   <autoFilter ref="A3:AM3" xr:uid="{A7555910-4F01-4A83-83B1-DAA1B4FA9702}"/>
   <mergeCells count="73">
+    <mergeCell ref="A13:D13"/>
+    <mergeCell ref="I8:I9"/>
+    <mergeCell ref="I10:I11"/>
+    <mergeCell ref="F2:F3"/>
+    <mergeCell ref="E4:E5"/>
+    <mergeCell ref="E6:E7"/>
+    <mergeCell ref="E8:E9"/>
+    <mergeCell ref="E10:E11"/>
+    <mergeCell ref="B4:B5"/>
+    <mergeCell ref="B6:B7"/>
+    <mergeCell ref="B8:B9"/>
+    <mergeCell ref="B10:B11"/>
+    <mergeCell ref="A10:A11"/>
+    <mergeCell ref="A8:A9"/>
+    <mergeCell ref="A6:A7"/>
+    <mergeCell ref="A4:A5"/>
+    <mergeCell ref="I6:I7"/>
+    <mergeCell ref="L4:L5"/>
+    <mergeCell ref="L6:L7"/>
+    <mergeCell ref="R4:R5"/>
+    <mergeCell ref="R6:R7"/>
+    <mergeCell ref="AK2:AM2"/>
+    <mergeCell ref="AH2:AJ2"/>
+    <mergeCell ref="AE2:AG2"/>
+    <mergeCell ref="AB2:AD2"/>
+    <mergeCell ref="I4:I5"/>
+    <mergeCell ref="Y2:AA2"/>
+    <mergeCell ref="V2:X2"/>
+    <mergeCell ref="S2:U2"/>
+    <mergeCell ref="P2:R2"/>
+    <mergeCell ref="M2:O2"/>
+    <mergeCell ref="J2:L2"/>
+    <mergeCell ref="AM4:AM5"/>
+    <mergeCell ref="G2:I2"/>
+    <mergeCell ref="L8:L9"/>
+    <mergeCell ref="L10:L11"/>
+    <mergeCell ref="O4:O5"/>
+    <mergeCell ref="O6:O7"/>
+    <mergeCell ref="O8:O9"/>
+    <mergeCell ref="O10:O11"/>
+    <mergeCell ref="R8:R9"/>
+    <mergeCell ref="R10:R11"/>
+    <mergeCell ref="U4:U5"/>
+    <mergeCell ref="U6:U7"/>
+    <mergeCell ref="U8:U9"/>
+    <mergeCell ref="U10:U11"/>
+    <mergeCell ref="AM6:AM7"/>
+    <mergeCell ref="AM8:AM9"/>
+    <mergeCell ref="AM10:AM11"/>
+    <mergeCell ref="AD4:AD5"/>
+    <mergeCell ref="AD6:AD7"/>
+    <mergeCell ref="AD8:AD9"/>
+    <mergeCell ref="AD10:AD11"/>
+    <mergeCell ref="AG4:AG5"/>
+    <mergeCell ref="AG6:AG7"/>
+    <mergeCell ref="AG8:AG9"/>
+    <mergeCell ref="AG10:AG11"/>
     <mergeCell ref="F10:F11"/>
     <mergeCell ref="F8:F9"/>
     <mergeCell ref="F6:F7"/>
@@ -2193,63 +2250,6 @@
     <mergeCell ref="AA6:AA7"/>
     <mergeCell ref="AA8:AA9"/>
     <mergeCell ref="AA10:AA11"/>
-    <mergeCell ref="AM6:AM7"/>
-    <mergeCell ref="AM8:AM9"/>
-    <mergeCell ref="AM10:AM11"/>
-    <mergeCell ref="AD4:AD5"/>
-    <mergeCell ref="AD6:AD7"/>
-    <mergeCell ref="AD8:AD9"/>
-    <mergeCell ref="AD10:AD11"/>
-    <mergeCell ref="AG4:AG5"/>
-    <mergeCell ref="AG6:AG7"/>
-    <mergeCell ref="AG8:AG9"/>
-    <mergeCell ref="AG10:AG11"/>
-    <mergeCell ref="R8:R9"/>
-    <mergeCell ref="R10:R11"/>
-    <mergeCell ref="U4:U5"/>
-    <mergeCell ref="U6:U7"/>
-    <mergeCell ref="U8:U9"/>
-    <mergeCell ref="U10:U11"/>
-    <mergeCell ref="L8:L9"/>
-    <mergeCell ref="L10:L11"/>
-    <mergeCell ref="O4:O5"/>
-    <mergeCell ref="O6:O7"/>
-    <mergeCell ref="O8:O9"/>
-    <mergeCell ref="O10:O11"/>
-    <mergeCell ref="AK2:AM2"/>
-    <mergeCell ref="AH2:AJ2"/>
-    <mergeCell ref="AE2:AG2"/>
-    <mergeCell ref="AB2:AD2"/>
-    <mergeCell ref="I4:I5"/>
-    <mergeCell ref="Y2:AA2"/>
-    <mergeCell ref="V2:X2"/>
-    <mergeCell ref="S2:U2"/>
-    <mergeCell ref="P2:R2"/>
-    <mergeCell ref="M2:O2"/>
-    <mergeCell ref="J2:L2"/>
-    <mergeCell ref="AM4:AM5"/>
-    <mergeCell ref="G2:I2"/>
-    <mergeCell ref="I6:I7"/>
-    <mergeCell ref="L4:L5"/>
-    <mergeCell ref="L6:L7"/>
-    <mergeCell ref="R4:R5"/>
-    <mergeCell ref="R6:R7"/>
-    <mergeCell ref="A13:D13"/>
-    <mergeCell ref="I8:I9"/>
-    <mergeCell ref="I10:I11"/>
-    <mergeCell ref="F2:F3"/>
-    <mergeCell ref="E4:E5"/>
-    <mergeCell ref="E6:E7"/>
-    <mergeCell ref="E8:E9"/>
-    <mergeCell ref="E10:E11"/>
-    <mergeCell ref="B4:B5"/>
-    <mergeCell ref="B6:B7"/>
-    <mergeCell ref="B8:B9"/>
-    <mergeCell ref="B10:B11"/>
-    <mergeCell ref="A10:A11"/>
-    <mergeCell ref="A8:A9"/>
-    <mergeCell ref="A6:A7"/>
-    <mergeCell ref="A4:A5"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>